<commit_message>
The files, methods and classes required for teacher and student login processes were completed and added to the project by obtaining the username and password from the excel file via Apache POI.
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelData/Campus_Data.xlsx
+++ b/src/test/java/ExcelData/Campus_Data.xlsx
@@ -1,31 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\Excel_Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D099983-D84E-47E8-95DF-60DEBF795C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="2070" windowWidth="13340" windowHeight="17130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>User Name</t>
   </si>
@@ -33,49 +22,388 @@
     <t>Password</t>
   </si>
   <si>
-    <t>turkeyts</t>
+    <t>teacher_1</t>
   </si>
   <si>
-    <t>TechnoStudy123</t>
+    <t>T12345</t>
+  </si>
+  <si>
+    <t>S10_11B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF008000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -83,28 +411,317 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -153,7 +770,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -188,7 +805,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -362,47 +979,51 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6285714285714" customWidth="1"/>
+    <col min="2" max="2" width="17.7238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="18.75" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="15.75" spans="1:2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12345</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>